<commit_message>
Sprint 4 Development and Issues fixed
</commit_message>
<xml_diff>
--- a/WEB_THEMES.war/ECOMMERCE_STD_TEMPLATE_V2/images/QuickCartExample.xlsx
+++ b/WEB_THEMES.war/ECOMMERCE_STD_TEMPLATE_V2/images/QuickCartExample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecommerce_ETNA\EcommerceRepository\WEB_THEMES.war\ECOMMERCE_STD_TEMPLATE_V2\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEP_HUB\EcommerceRepository\WEB_THEMES.war\ECOMMERCE_STD_TEMPLATE_V2\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Quantity</t>
+    <t>Cantidad</t>
   </si>
   <si>
-    <t>Key Word</t>
+    <t>Palabra clave</t>
   </si>
 </sst>
 </file>
@@ -379,16 +379,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -408,7 +406,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -420,7 +418,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>